<commit_message>
modified a Excel file. a little.
</commit_message>
<xml_diff>
--- a/source_tables.xlsx
+++ b/source_tables.xlsx
@@ -12,7 +12,8 @@
     <sheet name="table4.3" sheetId="3" r:id="rId3"/>
     <sheet name="table4.2" sheetId="4" r:id="rId4"/>
     <sheet name="table2.5" sheetId="6" r:id="rId5"/>
-    <sheet name="table2.1" sheetId="7" r:id="rId6"/>
+    <sheet name="table2.2" sheetId="8" r:id="rId6"/>
+    <sheet name="table2.1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="153">
   <si>
     <t>%read, %write</t>
     <phoneticPr fontId="1"/>
@@ -2557,6 +2558,164 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="0.83203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="0.83203125" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="12.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="5" customHeight="1">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4" ht="14">
+      <c r="A2" s="10"/>
+      <c r="B2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="4" customHeight="1">
+      <c r="A3" s="10"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" ht="14">
+      <c r="A4" s="10"/>
+      <c r="B4" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:4" ht="14">
+      <c r="A5" s="10"/>
+      <c r="B5" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" ht="14">
+      <c r="A6" s="10"/>
+      <c r="B6" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:4" ht="14">
+      <c r="A7" s="10"/>
+      <c r="B7" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:4" ht="14">
+      <c r="A8" s="10"/>
+      <c r="B8" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:4" ht="14">
+      <c r="A9" s="10"/>
+      <c r="B9" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:4" ht="14">
+      <c r="A10" s="10"/>
+      <c r="B10" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" ht="14">
+      <c r="A11" s="10"/>
+      <c r="B11" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:4" ht="14">
+      <c r="A12" s="10"/>
+      <c r="B12" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" ht="5" customHeight="1">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:4" ht="14">
+      <c r="A14" s="10"/>
+      <c r="B14" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B14:C14"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView showRuler="0" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="D14" sqref="A1:D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>